<commit_message>
[Fix]: exclusion of 8 redundant metrics
</commit_message>
<xml_diff>
--- a/experiments/verification/CMA_metrics.xlsx
+++ b/experiments/verification/CMA_metrics.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -50,12 +50,6 @@
     <t>Pearson</t>
   </si>
   <si>
-    <t>MBRAE</t>
-  </si>
-  <si>
-    <t>UMBRAE</t>
-  </si>
-  <si>
     <t>ME</t>
   </si>
   <si>
@@ -83,12 +77,6 @@
     <t>STDAE</t>
   </si>
   <si>
-    <t>STDAPE</t>
-  </si>
-  <si>
-    <t>RMSPE</t>
-  </si>
-  <si>
     <t>RMDSPE</t>
   </si>
   <si>
@@ -101,19 +89,7 @@
     <t>RRSE</t>
   </si>
   <si>
-    <t>MRE</t>
-  </si>
-  <si>
     <t>RAE</t>
-  </si>
-  <si>
-    <t>MRAE</t>
-  </si>
-  <si>
-    <t>MDRAE</t>
-  </si>
-  <si>
-    <t>GMRAE</t>
   </si>
   <si>
     <t>MDA</t>
@@ -474,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -609,7 +585,7 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>0.5763876984209183</v>
+        <v>0.004089308246898821</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -620,7 +596,7 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>1.360649103608045</v>
+        <v>0.02995354649144145</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -631,7 +607,7 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>0.004089308246898821</v>
+        <v>0.01295261329765343</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -642,7 +618,7 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>0.02995354649144145</v>
+        <v>0.01399247127988906</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -653,7 +629,7 @@
         <v>15</v>
       </c>
       <c r="C16">
-        <v>0.01295261329765343</v>
+        <v>-0.1323485138266888</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -664,7 +640,7 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <v>0.01399247127988906</v>
+        <v>0.01827765156078726</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -675,7 +651,7 @@
         <v>17</v>
       </c>
       <c r="C18">
-        <v>-0.1323485138266888</v>
+        <v>0.08431591626681864</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -686,7 +662,7 @@
         <v>18</v>
       </c>
       <c r="C19">
-        <v>0.01827765156078726</v>
+        <v>0.01814167522089438</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -697,7 +673,7 @@
         <v>19</v>
       </c>
       <c r="C20">
-        <v>0.08431591626681864</v>
+        <v>0.06979929874035952</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -708,7 +684,7 @@
         <v>20</v>
       </c>
       <c r="C21">
-        <v>0.01814167522089438</v>
+        <v>0.0182776516644037</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -719,7 +695,7 @@
         <v>21</v>
       </c>
       <c r="C22">
-        <v>0.06979929874035952</v>
+        <v>1.114828989925057</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -730,7 +706,7 @@
         <v>22</v>
       </c>
       <c r="C23">
-        <v>1.948225005831168</v>
+        <v>0.2435018244926589</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -741,7 +717,7 @@
         <v>23</v>
       </c>
       <c r="C24">
-        <v>1.921372183205107</v>
+        <v>0.2435018244926589</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -752,7 +728,7 @@
         <v>24</v>
       </c>
       <c r="C25">
-        <v>0.0182776516644037</v>
+        <v>0.1607764227743601</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -763,94 +739,6 @@
         <v>25</v>
       </c>
       <c r="C26">
-        <v>1.114828989925057</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27">
-        <v>0.2435018244926589</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28">
-        <v>0.2435018244926589</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29">
-        <v>-11323359.20968228</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30">
-        <v>0.1607764227743601</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31">
-        <v>11323377.69487423</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32">
-        <v>1.936122563707623</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33">
-        <v>1.790703747520231</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34">
         <v>0.8268251273344652</v>
       </c>
     </row>
@@ -861,7 +749,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -996,7 +884,7 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>0.4524685828586031</v>
+        <v>0.07806747448375632</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1007,7 +895,7 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>0.8263792153167999</v>
+        <v>0.08902083416939134</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1018,7 +906,7 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>0.07806747448375632</v>
+        <v>0.03374408246447243</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1029,7 +917,7 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>0.08902083416939134</v>
+        <v>0.03716715950063998</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1040,7 +928,7 @@
         <v>15</v>
       </c>
       <c r="C16">
-        <v>0.03374408246447243</v>
+        <v>0.06381245502859632</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1051,7 +939,7 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <v>0.03716715950063998</v>
+        <v>0.03023503284762205</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1062,7 +950,7 @@
         <v>17</v>
       </c>
       <c r="C18">
-        <v>0.06381245502859632</v>
+        <v>0.08764112327001099</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1073,7 +961,7 @@
         <v>18</v>
       </c>
       <c r="C19">
-        <v>0.03023503284762205</v>
+        <v>0.03054111059298797</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1084,7 +972,7 @@
         <v>19</v>
       </c>
       <c r="C20">
-        <v>0.08764112327001099</v>
+        <v>0.1372102913533303</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1095,7 +983,7 @@
         <v>20</v>
       </c>
       <c r="C21">
-        <v>0.03054111059298797</v>
+        <v>0.03023596363451101</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1106,7 +994,7 @@
         <v>21</v>
       </c>
       <c r="C22">
-        <v>0.1372102913533303</v>
+        <v>0.761527795877225</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1117,7 +1005,7 @@
         <v>22</v>
       </c>
       <c r="C23">
-        <v>0.1184445330907874</v>
+        <v>0.2545599390708055</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1128,7 +1016,7 @@
         <v>23</v>
       </c>
       <c r="C24">
-        <v>0.1334084934609991</v>
+        <v>0.2545599390708055</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1139,7 +1027,7 @@
         <v>24</v>
       </c>
       <c r="C25">
-        <v>0.03023596363451101</v>
+        <v>0.2282842640976591</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1150,94 +1038,6 @@
         <v>25</v>
       </c>
       <c r="C26">
-        <v>0.761527795877225</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27">
-        <v>0.2545599390708055</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28">
-        <v>0.2545599390708055</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29">
-        <v>26464379.7629247</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30">
-        <v>0.2282842640976591</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31">
-        <v>26464385.49377708</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32">
-        <v>0.7160210105861469</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33">
-        <v>0.7466065411084692</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34">
         <v>0.8404074702886248</v>
       </c>
     </row>

</xml_diff>